<commit_message>
add cluster rename script
</commit_message>
<xml_diff>
--- a/src/unique_clusters_comparison.xlsx
+++ b/src/unique_clusters_comparison.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,445 +453,172 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MeV.2.1</t>
+          <t>Imm.0.8.1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MeV.2.1</t>
+          <t>Imm.0.8.1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MeV.2.1</t>
+          <t>Imm.0.8.1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MeV.2.8</t>
+          <t>Imm.0.8.2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MeV.2.8</t>
+          <t>Imm.0.8.2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MeV.2.8</t>
+          <t>Imm.0.8.2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MeV.1.4.2</t>
+          <t>Imm.0.8.0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MeV.1.4.2</t>
+          <t>Imm.0.8.0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MeV.1.4.2</t>
+          <t>Imm.0.8.0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MeV.4.21</t>
+          <t>Imm.1.2.13</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MeV.4.21</t>
+          <t>Imm.1.2.13</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MeV.4.21</t>
+          <t>Imm.1.2.13</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MeV.1.4.5</t>
+          <t>Imm.1.2.4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MeV.1.4.5</t>
+          <t>Imm.1.2.4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MeV.1.4.5</t>
+          <t>Imm.1.2.4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MeV.1.4.7</t>
+          <t>Imm.0.8.6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MeV.1.4.7</t>
+          <t>Imm.0.8.6</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MeV.1.4.7</t>
+          <t>Imm.0.8.6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MeV.1.4.15</t>
+          <t>Imm.1.2.5</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MeV.1.4.15</t>
+          <t>Imm.1.2.5</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MeV.1.4.15</t>
+          <t>Imm.1.2.5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MeV.1.4.6</t>
+          <t>Imm.1.2.12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MeV.1.4.6</t>
+          <t>Imm.1.2.12</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MeV.1.4.6</t>
+          <t>Imm.1.2.12</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MeV.1.4.4</t>
+          <t>Imm.1.2.15</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MeV.1.4.4</t>
+          <t>Imm.1.2.15</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MeV.1.4.4</t>
+          <t>Imm.1.2.15</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MeV.1.4.20</t>
+          <t>Imm.NA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MeV.1.4.20</t>
+          <t>Imm.NA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MeV.1.4.20</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>MeV.1.4.1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MeV.1.4.1</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>MeV.1.4.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>MeV.1.4.11</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>MeV.1.4.11</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>MeV.1.4.11</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>MeV.1.4.8</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>MeV.1.4.8</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>MeV.1.4.8</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>MeV.4.12</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>MeV.4.12</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>MeV.4.12</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>MeV.4.4</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>MeV.4.4</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>MeV.4.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MeV.1.4.0</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>MeV.3.17</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>MeV.3.17</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>MeV.3.17</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>MeV.4.31</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>MeV.4.31</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>MeV.4.31</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>MeV.4.1</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>MeV.4.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>MeV.4.1</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>MeV.4.34</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MeV.4.34</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>MeV.4.34</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>MeV.1.4.13</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>MeV.1.4.13</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>MeV.1.4.13</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>MeV.3.30</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>MeV.3.30</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>MeV.3.30</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>MeV.4.26</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>MeV.4.26</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>MeV.4.26</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>MeV.NA</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>MeV.NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>MeV.1.4.12</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>MeV.1.4.21</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>MeV.1.4.21</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>MeV.1.4.21</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>MeV.4.30</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>MeV.4.30</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>MeV.4.30</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>MeV.NA</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
+          <t>Imm.NA</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add new Neuron scripts
</commit_message>
<xml_diff>
--- a/src/unique_clusters_comparison.xlsx
+++ b/src/unique_clusters_comparison.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,151 +441,31 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>leiden_fusion</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Imm.0.8.1</t>
+          <t>Neu.1.5.47</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Imm.0.8.1</t>
+          <t>Neu.CSFcN.0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Imm.0.8.2</t>
+          <t>Neu.5.81</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Imm.0.8.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Imm.0.8.0</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Imm.0.8.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Imm.1.2.13</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Imm.1.2.13</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Imm.1.2.4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Imm.1.2.4</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Imm.0.8.6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Imm.0.8.6</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Imm.1.2.14</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Imm.1.2.14</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Imm.1.2.5</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Imm.1.2.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Imm.1.2.12</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Imm.1.2.12</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Imm.0.8.3</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Imm.0.8.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Imm.1.2.15</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Imm.1.2.15</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Imm.NA</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Imm.NA</t>
+          <t>Neu.Epend.0</t>
         </is>
       </c>
     </row>

</xml_diff>